<commit_message>
last change before hosting
</commit_message>
<xml_diff>
--- a/conception.xlsx
+++ b/conception.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t xml:space="preserve">Application de séléction de régime selon besoin</t>
   </si>
@@ -46,7 +46,10 @@
     <t xml:space="preserve">CheckList</t>
   </si>
   <si>
-    <t xml:space="preserve">Inscription</t>
+    <t xml:space="preserve">Kael</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inscription -------------done</t>
   </si>
   <si>
     <t xml:space="preserve">fonction inscription</t>
@@ -55,7 +58,7 @@
     <t xml:space="preserve">table User</t>
   </si>
   <si>
-    <t xml:space="preserve">Login</t>
+    <t xml:space="preserve">Login -------------------done</t>
   </si>
   <si>
     <t xml:space="preserve">fonction checkLogin</t>
@@ -70,7 +73,7 @@
     <t xml:space="preserve">fonction completionProfil</t>
   </si>
   <si>
-    <t xml:space="preserve">Objectif</t>
+    <t xml:space="preserve">Objectif-----------------done</t>
   </si>
   <si>
     <t xml:space="preserve">fonction choixObjectif</t>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">table Objectif</t>
   </si>
   <si>
+    <t xml:space="preserve">Mahery</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choix regime</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
     <t xml:space="preserve">table Régime</t>
   </si>
   <si>
+    <t xml:space="preserve">CRUD Plat</t>
+  </si>
+  <si>
     <t xml:space="preserve">fonction chercherRegimeApproprié</t>
   </si>
   <si>
@@ -103,6 +112,9 @@
     <t xml:space="preserve">fonction chercherActiviteApproprié</t>
   </si>
   <si>
+    <t xml:space="preserve">Anouchka</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rajout d’argent</t>
   </si>
   <si>
@@ -110,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">table Wallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction CRUD Money</t>
   </si>
   <si>
     <t xml:space="preserve">fonction addMoney</t>
@@ -188,28 +203,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,13 +249,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.59"/>
@@ -279,37 +298,52 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="n">
         <v>20</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="4" t="n">
@@ -317,101 +351,172 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B8" s="3"/>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="2" t="n">
         <v>20</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="s">
-        <v>19</v>
+      <c r="A10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>30</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5"/>
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="2" t="n">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="2" t="n">
         <v>30</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3"/>
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E13" s="2" t="n">
         <v>30</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="2" t="n">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3"/>
+      <c r="A15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E15" s="2" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="2"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -419,12 +524,12 @@
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D15:D17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>